<commit_message>
Avances en creación de vistas, procedimientos y triggers
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcorrea\Desktop\Salchy\UTN\Bases de Datos II\TP-integrador-dbii\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Salchy\UTN\Cursada 2025\Base de Datos II\TP-integrador-dbii\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8325297-A98E-4AA6-8788-2AA9914F2359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4D8B03-A8F0-4216-818A-A25EFF9659BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6570" yWindow="2895" windowWidth="17715" windowHeight="10665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Requisitos</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Mostrar contenido de una venta</t>
   </si>
   <si>
-    <t>Debería mostrar todos los artículos que formaron parte de una venta</t>
-  </si>
-  <si>
     <t>Realizar un alta de artículo</t>
   </si>
   <si>
@@ -90,7 +87,30 @@
     <t>Debería descontar el stock del producto que se vendió</t>
   </si>
   <si>
-    <t>Sería un AFTER UPDATE</t>
+    <t>Encargado de la tarea</t>
+  </si>
+  <si>
+    <t>Debería mostrar todos los artículos que formaron parte de una venta
+Join entre Ventas, ArtículoVenta y Artículo para obtener el nombre del artículo</t>
+  </si>
+  <si>
+    <t>Leandro Correa</t>
+  </si>
+  <si>
+    <t>Facundo</t>
+  </si>
+  <si>
+    <t>Promedio de importe de ventas
+Tabla Ventas con AVG de importeTotal</t>
+  </si>
+  <si>
+    <t>Mostrar el promedio de ventas realizadas</t>
+  </si>
+  <si>
+    <t>Sería un AFTER UPDATE, de la tabla Artículos</t>
+  </si>
+  <si>
+    <t>Jesus</t>
   </si>
 </sst>
 </file>
@@ -126,16 +146,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -165,18 +194,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26208452-FD88-4DC2-804A-C1CFD2921A16}" name="Tabla2" displayName="Tabla2" ref="A1:D9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:D9" xr:uid="{26208452-FD88-4DC2-804A-C1CFD2921A16}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26208452-FD88-4DC2-804A-C1CFD2921A16}" name="Tabla2" displayName="Tabla2" ref="A1:E9" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E9" xr:uid="{26208452-FD88-4DC2-804A-C1CFD2921A16}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="4">
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{3C7CA349-29B2-4BA7-A517-1C7EC9E6A53B}" name="Requisitos" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{E21B31FD-869B-4C8D-8A5D-289621B18FF9}" name="Descripcion" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{07906AA6-ADC7-4C8F-8C81-6D6137F3AA0E}" name="Comentarios" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{A096697E-A77D-43C5-AD72-203D218D6077}" name="Cumplido"/>
+    <tableColumn id="4" xr3:uid="{A096697E-A77D-43C5-AD72-203D218D6077}" name="Cumplido" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{ED30E2ED-B2C4-4D67-AD9E-593199E41A83}" name="Encargado de la tarea" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -445,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,10 +487,11 @@
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="90.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,11 +501,14 @@
       <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -483,64 +518,83 @@
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -548,6 +602,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Iserción manual de ventas, para probar la vista creada
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Salchy\UTN\Cursada 2025\Base de Datos II\TP-integrador-dbii\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcorrea\Desktop\Salchy\UTN\Bases de Datos II\TP-integrador-dbii\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4D8B03-A8F0-4216-818A-A25EFF9659BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F899092-F8E3-4A73-97C6-AF093466F5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="2895" windowWidth="17715" windowHeight="10665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Requisitos</t>
   </si>
@@ -79,12 +79,6 @@
   </si>
   <si>
     <t>Modificar el stock cuando se ingresa un artículo</t>
-  </si>
-  <si>
-    <t>Realizar una venta</t>
-  </si>
-  <si>
-    <t>Debería descontar el stock del producto que se vendió</t>
   </si>
   <si>
     <t>Encargado de la tarea</t>
@@ -111,6 +105,19 @@
   </si>
   <si>
     <t>Jesus</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Registrar una venta de un artículo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debería descontar el stock del producto que se vendió
+Es un insert a ArticuloVentas, pasandole por argumento, el ID de venta al que va asociado ese artículo
+Para hacerlo más sencillo, vamos a realizar un procedimiento, de registrar un ítem de venta, para una venta en cuestión
+A tener en cuenta: se deberá guardar el precio del artículo en el campo importeUnitario,para guardar el precio de esa venta, así poder modificar el precio luego de ese artículo, sin que influya en los reportes, ya que el precio de venta es otro.
+A demas, si la cantidad a comprar, es mayor a la del stock que hay disponible, arrojar error </t>
   </si>
 </sst>
 </file>
@@ -478,15 +485,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="90.7109375" customWidth="1"/>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="108.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
   </cols>
@@ -505,7 +512,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -519,7 +526,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -530,10 +537,13 @@
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -541,13 +551,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -558,21 +568,26 @@
         <v>16</v>
       </c>
       <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -582,7 +597,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1"/>
     </row>

</xml_diff>

<commit_message>
Avances en procedimientos, y añadido de bloques de transacciones para mejor control
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcorrea\Desktop\Salchy\UTN\Bases de Datos II\TP-integrador-dbii\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F899092-F8E3-4A73-97C6-AF093466F5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DC2EC2-8F58-41ED-9098-32D290F1F0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Requisitos</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Mostrar el stock que hay disponible</t>
-  </si>
-  <si>
-    <t>Debería devolver un listado con el stock que hay actualmente (un join entre Articulos y Stock)</t>
   </si>
   <si>
     <t>Mostrar contenido de una venta</t>
@@ -99,9 +96,6 @@
   </si>
   <si>
     <t>Mostrar el promedio de ventas realizadas</t>
-  </si>
-  <si>
-    <t>Sería un AFTER UPDATE, de la tabla Artículos</t>
   </si>
   <si>
     <t>Jesus</t>
@@ -118,6 +112,18 @@
 Para hacerlo más sencillo, vamos a realizar un procedimiento, de registrar un ítem de venta, para una venta en cuestión
 A tener en cuenta: se deberá guardar el precio del artículo en el campo importeUnitario,para guardar el precio de esa venta, así poder modificar el precio luego de ese artículo, sin que influya en los reportes, ya que el precio de venta es otro.
 A demas, si la cantidad a comprar, es mayor a la del stock que hay disponible, arrojar error </t>
+  </si>
+  <si>
+    <t>Debería devolver un listado con el stock que hay actualmente (un join entre Articulos y Stock) Quizá sea un Left Join de Artículos con Stock, para que muestre todos los artículos, tengan stock o no</t>
+  </si>
+  <si>
+    <t>Modificar el importe de la venta al hacer un update de la tabla ArticuloVenta</t>
+  </si>
+  <si>
+    <t>SP_CargarStock(idArticulo, cantidad) Sería un AFTER UPDATE, de la tabla Artículos</t>
+  </si>
+  <si>
+    <t>AFTER UPDATE de la tabla ArticuloVenta, va a modificar la columna importeTotal de la tabla Ventas</t>
   </si>
 </sst>
 </file>
@@ -483,17 +489,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="108.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.140625" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
   </cols>
@@ -512,7 +518,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -522,11 +528,11 @@
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -534,16 +540,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -551,13 +557,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -565,14 +571,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -580,13 +586,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -594,10 +600,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -605,8 +611,12 @@
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -617,7 +627,15 @@
         <v>12</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Acomodo de ficheros, y fix en procedimientos, generación de datos a travez de los procedimientos, y prueba de vistas
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcorrea\Desktop\Salchy\UTN\Bases de Datos II\TP-integrador-dbii\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DC2EC2-8F58-41ED-9098-32D290F1F0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB7D2BB-5F34-47DF-ACFD-EA87EB256B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Requisitos</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Realizar un alta de artículo</t>
-  </si>
-  <si>
-    <t>Modificar el stock cuando se ingresa un artículo</t>
   </si>
   <si>
     <t>Encargado de la tarea</t>
@@ -117,13 +114,13 @@
     <t>Debería devolver un listado con el stock que hay actualmente (un join entre Articulos y Stock) Quizá sea un Left Join de Artículos con Stock, para que muestre todos los artículos, tengan stock o no</t>
   </si>
   <si>
-    <t>Modificar el importe de la venta al hacer un update de la tabla ArticuloVenta</t>
-  </si>
-  <si>
-    <t>SP_CargarStock(idArticulo, cantidad) Sería un AFTER UPDATE, de la tabla Artículos</t>
-  </si>
-  <si>
-    <t>AFTER UPDATE de la tabla ArticuloVenta, va a modificar la columna importeTotal de la tabla Ventas</t>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Modificar el importe de la venta al hacer un insert de la tabla ArticuloVenta</t>
+  </si>
+  <si>
+    <t>AFTER INSERT de la tabla ArticuloVenta, va a modificar la columna importeTotal de la tabla Ventas, para el Idventa</t>
   </si>
 </sst>
 </file>
@@ -491,15 +488,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="98.140625" customWidth="1"/>
+    <col min="3" max="3" width="103.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
   </cols>
@@ -518,7 +515,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -529,10 +526,13 @@
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -543,13 +543,13 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -557,13 +557,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -575,36 +575,35 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>26</v>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -615,7 +614,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -628,7 +627,7 @@
       </c>
       <c r="C9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Acomodo de proyecto + fix formato de fecha en db
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcorrea\Desktop\Salchy\UTN\Bases de Datos II\TP-integrador-dbii\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Salchy\UTN\Cursada 2025\Base de Datos II\TP-integrador-dbii\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB7D2BB-5F34-47DF-ACFD-EA87EB256B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA7B02F-5E33-45C0-9C06-7447090628D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Requisitos</t>
   </si>
@@ -489,7 +489,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,6 +562,9 @@
       <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Añadido de procedure 4, reacomodo de insert de datos, y reacomodo del proyecto
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Salchy\UTN\Cursada 2025\Base de Datos II\TP-integrador-dbii\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA7B02F-5E33-45C0-9C06-7447090628D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8AA29D-1264-49F2-8A1B-6CCCE0F801D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Requisitos</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Mostrar el stock que hay disponible</t>
-  </si>
-  <si>
-    <t>Mostrar contenido de una venta</t>
   </si>
   <si>
     <t>Realizar un alta de artículo</t>
@@ -114,13 +111,28 @@
     <t>Debería devolver un listado con el stock que hay actualmente (un join entre Articulos y Stock) Quizá sea un Left Join de Artículos con Stock, para que muestre todos los artículos, tengan stock o no</t>
   </si>
   <si>
-    <t>ok</t>
-  </si>
-  <si>
     <t>Modificar el importe de la venta al hacer un insert de la tabla ArticuloVenta</t>
   </si>
   <si>
     <t>AFTER INSERT de la tabla ArticuloVenta, va a modificar la columna importeTotal de la tabla Ventas, para el Idventa</t>
+  </si>
+  <si>
+    <t>Mostrar contenido de las ventas</t>
+  </si>
+  <si>
+    <t>Procedimiento 3</t>
+  </si>
+  <si>
+    <t>Realizar apertura de una venta</t>
+  </si>
+  <si>
+    <t>Procedimiento 4</t>
+  </si>
+  <si>
+    <t>Realizar modificación de stock</t>
+  </si>
+  <si>
+    <t>Realiza un UPDATE, recibe 2 argumentos, (idProducto, Cantidad)</t>
   </si>
 </sst>
 </file>
@@ -204,8 +216,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26208452-FD88-4DC2-804A-C1CFD2921A16}" name="Tabla2" displayName="Tabla2" ref="A1:E9" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E9" xr:uid="{26208452-FD88-4DC2-804A-C1CFD2921A16}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26208452-FD88-4DC2-804A-C1CFD2921A16}" name="Tabla2" displayName="Tabla2" ref="A1:E11" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E11" xr:uid="{26208452-FD88-4DC2-804A-C1CFD2921A16}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -486,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +527,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -526,13 +538,13 @@
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -540,16 +552,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -557,16 +569,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -574,70 +586,107 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reorden de proyecto y modificación de algunos procedures
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Salchy\UTN\Cursada 2025\Base de Datos II\TP-integrador-dbii\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8AA29D-1264-49F2-8A1B-6CCCE0F801D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD17A48-F7F0-4C9C-81A2-8979312A604D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>Requisitos</t>
   </si>
@@ -133,6 +133,30 @@
   </si>
   <si>
     <t>Realiza un UPDATE, recibe 2 argumentos, (idProducto, Cantidad)</t>
+  </si>
+  <si>
+    <t>Procedimiento 5</t>
+  </si>
+  <si>
+    <t>Realizar alta de Marca</t>
+  </si>
+  <si>
+    <t>Realizar insert de marca</t>
+  </si>
+  <si>
+    <t>Vista 4</t>
+  </si>
+  <si>
+    <t>Mostrar articulos con stock bajo</t>
+  </si>
+  <si>
+    <t>Leandro / Facundo</t>
+  </si>
+  <si>
+    <t>Notificación de productos con stok bajo</t>
+  </si>
+  <si>
+    <t>EN CURSO</t>
   </si>
 </sst>
 </file>
@@ -216,8 +240,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26208452-FD88-4DC2-804A-C1CFD2921A16}" name="Tabla2" displayName="Tabla2" ref="A1:E11" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E11" xr:uid="{26208452-FD88-4DC2-804A-C1CFD2921A16}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26208452-FD88-4DC2-804A-C1CFD2921A16}" name="Tabla2" displayName="Tabla2" ref="A1:E13" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E13" xr:uid="{26208452-FD88-4DC2-804A-C1CFD2921A16}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -498,16 +522,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="103.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
@@ -583,29 +607,27 @@
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
         <v>22</v>
       </c>
@@ -615,78 +637,116 @@
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="E11" s="1" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="E12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>